<commit_message>
Completed first draft of the feed
</commit_message>
<xml_diff>
--- a/2022-06-20/Run Times.xlsx
+++ b/2022-06-20/Run Times.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rohan/Git/TAPS-GTFS/2022-06-20/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rohan\Desktop\Git\TAPS-GTFS\2022-06-20\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD5E749-A0D2-5443-A49C-C67F92DF6838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{382AA785-C112-479D-A37A-C45F0729D938}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="460" windowWidth="21660" windowHeight="16080" xr2:uid="{45B10C95-EE45-9545-9559-471A854BF09A}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11265" xr2:uid="{45B10C95-EE45-9545-9559-471A854BF09A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +23,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -31,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Trip Time</t>
   </si>
@@ -70,6 +74,30 @@
   </si>
   <si>
     <t>Cowell to Main Gate</t>
+  </si>
+  <si>
+    <t>EG Loop</t>
+  </si>
+  <si>
+    <t>Main Gt to Cowell</t>
+  </si>
+  <si>
+    <t>Cowell to Sci Hill</t>
+  </si>
+  <si>
+    <t>Sci Hill to Oakes</t>
+  </si>
+  <si>
+    <t>Oakes to Main Gt</t>
+  </si>
+  <si>
+    <t>All Times</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
@@ -165,14 +193,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="46" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="21" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,15 +516,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1C498A5-26F4-944A-9B4E-C2BFE611477F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -540,7 +568,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0.2951388888888889</v>
       </c>
@@ -559,32 +587,32 @@
       <c r="F2" s="2">
         <v>3.7351851851851854</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2">
         <v>2375</v>
       </c>
-      <c r="J2" s="8">
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="K2" s="13">
+      <c r="K2" s="11">
         <v>0.3125</v>
       </c>
-      <c r="L2" s="13">
+      <c r="L2" s="11">
         <v>0.40277777777777773</v>
       </c>
-      <c r="M2" s="13">
+      <c r="M2" s="11">
         <v>0.4861111111111111</v>
       </c>
-      <c r="N2" s="13">
-        <v>0.52083333333333337</v>
-      </c>
-      <c r="O2" s="13">
-        <v>0</v>
-      </c>
-      <c r="P2" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N2" s="11">
+        <v>0.70138888888888884</v>
+      </c>
+      <c r="O2" s="11">
+        <v>0</v>
+      </c>
+      <c r="P2" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.31597222222222221</v>
       </c>
@@ -603,38 +631,38 @@
       <c r="F3" s="3">
         <v>3.8777777777777778</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3">
         <v>2374</v>
       </c>
-      <c r="J3" s="8">
-        <v>0</v>
-      </c>
-      <c r="K3" s="9">
-        <f>K2+(K5-K2)*0.33</f>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8">
+        <f t="shared" ref="K3:P3" si="0">K2+(K5-K2)*0.33</f>
         <v>0.31307291666666665</v>
       </c>
-      <c r="L3" s="9">
-        <f>L2+(L5-L2)*0.33</f>
+      <c r="L3" s="8">
+        <f t="shared" si="0"/>
         <v>0.40338888888888885</v>
       </c>
-      <c r="M3" s="9">
-        <f>M2+(M5-M2)*0.33</f>
+      <c r="M3" s="8">
+        <f t="shared" si="0"/>
         <v>0.48668402777777775</v>
       </c>
-      <c r="N3" s="9">
-        <f>N2+(N5-N2)*0.33</f>
-        <v>0.52152083333333332</v>
-      </c>
-      <c r="O3" s="9">
-        <f>O2+(O5-O2)*0.33</f>
+      <c r="N3" s="8">
+        <f t="shared" si="0"/>
+        <v>0.70207638888888879</v>
+      </c>
+      <c r="O3" s="8">
+        <f t="shared" si="0"/>
         <v>5.7291666666666667E-4</v>
       </c>
-      <c r="P3" s="9">
-        <f>P2+(P5-P2)*0.33</f>
+      <c r="P3" s="8">
+        <f t="shared" si="0"/>
         <v>5.7291666666666667E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.33680555555555558</v>
       </c>
@@ -653,38 +681,38 @@
       <c r="F4" s="3">
         <v>3.7166666666666668</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4">
         <v>1385</v>
       </c>
-      <c r="J4" s="8">
-        <v>0</v>
-      </c>
-      <c r="K4" s="9">
-        <f>K2+(K5-K2)*0.67</f>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4" s="8">
+        <f t="shared" ref="K4:P4" si="1">K2+(K5-K2)*0.67</f>
         <v>0.31366319444444446</v>
       </c>
-      <c r="L4" s="9">
-        <f>L2+(L5-L2)*0.67</f>
+      <c r="L4" s="8">
+        <f t="shared" si="1"/>
         <v>0.40401851851851844</v>
       </c>
-      <c r="M4" s="9">
-        <f>M2+(M5-M2)*0.67</f>
+      <c r="M4" s="8">
+        <f t="shared" si="1"/>
         <v>0.48727430555555556</v>
       </c>
-      <c r="N4" s="9">
-        <f>N2+(N5-N2)*0.67</f>
-        <v>0.52222916666666674</v>
-      </c>
-      <c r="O4" s="9">
-        <f>O2+(O5-O2)*0.67</f>
+      <c r="N4" s="8">
+        <f t="shared" si="1"/>
+        <v>0.70278472222222221</v>
+      </c>
+      <c r="O4" s="8">
+        <f t="shared" si="1"/>
         <v>1.1631944444444443E-3</v>
       </c>
-      <c r="P4" s="9">
-        <f>P2+(P5-P2)*0.67</f>
+      <c r="P4" s="8">
+        <f t="shared" si="1"/>
         <v>1.1631944444444443E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.3576388888888889</v>
       </c>
@@ -703,38 +731,38 @@
       <c r="F5" s="3">
         <v>3.6018518518518521</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5">
         <v>2670</v>
       </c>
-      <c r="J5" s="8">
+      <c r="J5">
         <v>1</v>
       </c>
-      <c r="K5" s="9">
-        <f>K2+C41</f>
+      <c r="K5" s="8">
+        <f t="shared" ref="K5:P5" si="2">K2+C41</f>
         <v>0.3142361111111111</v>
       </c>
-      <c r="L5" s="9">
-        <f>L2+D41</f>
+      <c r="L5" s="8">
+        <f t="shared" si="2"/>
         <v>0.40462962962962956</v>
       </c>
-      <c r="M5" s="9">
-        <f>M2+E41</f>
+      <c r="M5" s="8">
+        <f t="shared" si="2"/>
         <v>0.48784722222222221</v>
       </c>
-      <c r="N5" s="9">
-        <f>N2+F41</f>
-        <v>0.5229166666666667</v>
-      </c>
-      <c r="O5" s="9">
-        <f>O2+G41</f>
+      <c r="N5" s="8">
+        <f t="shared" si="2"/>
+        <v>0.70347222222222217</v>
+      </c>
+      <c r="O5" s="8">
+        <f t="shared" si="2"/>
         <v>1.736111111111111E-3</v>
       </c>
-      <c r="P5" s="9">
-        <f>P2+H41</f>
+      <c r="P5" s="8">
+        <f t="shared" si="2"/>
         <v>1.736111111111111E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>0.37847222222222227</v>
       </c>
@@ -753,38 +781,38 @@
       <c r="F6" s="3">
         <v>3.875</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6">
         <v>2671</v>
       </c>
-      <c r="J6" s="8">
-        <v>0</v>
-      </c>
-      <c r="K6" s="9">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6" s="8">
         <f>K5+(K9-K5)*0.25</f>
         <v>0.31501736111111112</v>
       </c>
-      <c r="L6" s="9">
-        <f t="shared" ref="L6:P6" si="0">L5+(L9-L5)*0.25</f>
+      <c r="L6" s="8">
+        <f t="shared" ref="L6:P6" si="3">L5+(L9-L5)*0.25</f>
         <v>0.405324074074074</v>
       </c>
-      <c r="M6" s="9">
-        <f t="shared" si="0"/>
+      <c r="M6" s="8">
+        <f t="shared" si="3"/>
         <v>0.48851273148148144</v>
       </c>
-      <c r="N6" s="9">
-        <f t="shared" si="0"/>
-        <v>0.52361111111111114</v>
-      </c>
-      <c r="O6" s="9">
-        <f t="shared" si="0"/>
+      <c r="N6" s="8">
+        <f t="shared" si="3"/>
+        <v>0.70416666666666661</v>
+      </c>
+      <c r="O6" s="8">
+        <f t="shared" si="3"/>
         <v>2.3437499999999999E-3</v>
       </c>
-      <c r="P6" s="9">
-        <f t="shared" si="0"/>
+      <c r="P6" s="8">
+        <f t="shared" si="3"/>
         <v>2.3437499999999999E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>0.39930555555555558</v>
       </c>
@@ -803,38 +831,38 @@
       <c r="F7" s="4">
         <v>3.4277777777777776</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7">
         <v>2672</v>
       </c>
-      <c r="J7" s="8">
-        <v>0</v>
-      </c>
-      <c r="K7" s="9">
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="8">
         <f>K5+(K9-K5)*0.5</f>
         <v>0.31579861111111107</v>
       </c>
-      <c r="L7" s="9">
-        <f t="shared" ref="L7:P7" si="1">L5+(L9-L5)*0.5</f>
+      <c r="L7" s="8">
+        <f t="shared" ref="L7:P7" si="4">L5+(L9-L5)*0.5</f>
         <v>0.40601851851851845</v>
       </c>
-      <c r="M7" s="9">
-        <f t="shared" si="1"/>
+      <c r="M7" s="8">
+        <f t="shared" si="4"/>
         <v>0.48917824074074073</v>
       </c>
-      <c r="N7" s="9">
-        <f t="shared" si="1"/>
-        <v>0.52430555555555558</v>
-      </c>
-      <c r="O7" s="9">
-        <f t="shared" si="1"/>
+      <c r="N7" s="8">
+        <f t="shared" si="4"/>
+        <v>0.70486111111111105</v>
+      </c>
+      <c r="O7" s="8">
+        <f t="shared" si="4"/>
         <v>2.9513888888888888E-3</v>
       </c>
-      <c r="P7" s="9">
-        <f t="shared" si="1"/>
+      <c r="P7" s="8">
+        <f t="shared" si="4"/>
         <v>2.9513888888888888E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>0.4201388888888889</v>
       </c>
@@ -853,38 +881,38 @@
       <c r="F8" s="4">
         <v>3.6259259259259258</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8">
         <v>2673</v>
       </c>
-      <c r="J8" s="8">
-        <v>0</v>
-      </c>
-      <c r="K8" s="9">
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8" s="8">
         <f>K5+(K9-K5)*0.75</f>
         <v>0.31657986111111108</v>
       </c>
-      <c r="L8" s="9">
-        <f t="shared" ref="L8:P8" si="2">L5+(L9-L5)*0.75</f>
+      <c r="L8" s="8">
+        <f t="shared" ref="L8:P8" si="5">L5+(L9-L5)*0.75</f>
         <v>0.40671296296296289</v>
       </c>
-      <c r="M8" s="9">
-        <f t="shared" si="2"/>
+      <c r="M8" s="8">
+        <f t="shared" si="5"/>
         <v>0.48984375000000002</v>
       </c>
-      <c r="N8" s="9">
-        <f t="shared" si="2"/>
-        <v>0.52500000000000002</v>
-      </c>
-      <c r="O8" s="9">
-        <f t="shared" si="2"/>
+      <c r="N8" s="8">
+        <f t="shared" si="5"/>
+        <v>0.70555555555555549</v>
+      </c>
+      <c r="O8" s="8">
+        <f t="shared" si="5"/>
         <v>3.5590277777777777E-3</v>
       </c>
-      <c r="P8" s="9">
-        <f t="shared" si="2"/>
+      <c r="P8" s="8">
+        <f t="shared" si="5"/>
         <v>3.5590277777777777E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0.44097222222222227</v>
       </c>
@@ -903,38 +931,38 @@
       <c r="F9" s="4">
         <v>3.6703703703703705</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9">
         <v>2674</v>
       </c>
-      <c r="J9" s="8">
+      <c r="J9">
         <v>1</v>
       </c>
-      <c r="K9" s="9">
-        <f>K5+C42</f>
+      <c r="K9" s="8">
+        <f t="shared" ref="K9:P9" si="6">K5+C42</f>
         <v>0.31736111111111109</v>
       </c>
-      <c r="L9" s="9">
-        <f>L5+D42</f>
+      <c r="L9" s="8">
+        <f t="shared" si="6"/>
         <v>0.40740740740740733</v>
       </c>
-      <c r="M9" s="9">
-        <f>M5+E42</f>
+      <c r="M9" s="8">
+        <f t="shared" si="6"/>
         <v>0.49050925925925926</v>
       </c>
-      <c r="N9" s="9">
-        <f>N5+F42</f>
-        <v>0.52569444444444446</v>
-      </c>
-      <c r="O9" s="9">
-        <f>O5+G42</f>
+      <c r="N9" s="8">
+        <f t="shared" si="6"/>
+        <v>0.70624999999999993</v>
+      </c>
+      <c r="O9" s="8">
+        <f t="shared" si="6"/>
         <v>4.1666666666666666E-3</v>
       </c>
-      <c r="P9" s="9">
-        <f>P5+H42</f>
+      <c r="P9" s="8">
+        <f t="shared" si="6"/>
         <v>4.1666666666666666E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>0.46180555555555558</v>
       </c>
@@ -953,38 +981,38 @@
       <c r="F10" s="4">
         <v>3.9722222222222223</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10">
         <v>2675</v>
       </c>
-      <c r="J10" s="8">
-        <v>0</v>
-      </c>
-      <c r="K10" s="9">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10" s="8">
         <f>K9+(K11-K9)*0.3</f>
         <v>0.3178819444444444</v>
       </c>
-      <c r="L10" s="9">
-        <f t="shared" ref="L10:P10" si="3">L9+(L11-L9)*0.3</f>
+      <c r="L10" s="8">
+        <f t="shared" ref="L10:P10" si="7">L9+(L11-L9)*0.3</f>
         <v>0.40792824074074063</v>
       </c>
-      <c r="M10" s="9">
-        <f t="shared" si="3"/>
+      <c r="M10" s="8">
+        <f t="shared" si="7"/>
         <v>0.49113425925925924</v>
       </c>
-      <c r="N10" s="9">
-        <f t="shared" si="3"/>
-        <v>0.52621527777777777</v>
-      </c>
-      <c r="O10" s="9">
-        <f t="shared" si="3"/>
+      <c r="N10" s="8">
+        <f t="shared" si="7"/>
+        <v>0.70677083333333324</v>
+      </c>
+      <c r="O10" s="8">
+        <f t="shared" si="7"/>
         <v>4.6874999999999998E-3</v>
       </c>
-      <c r="P10" s="9">
-        <f t="shared" si="3"/>
+      <c r="P10" s="8">
+        <f t="shared" si="7"/>
         <v>4.5833333333333334E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>0.4826388888888889</v>
       </c>
@@ -1003,38 +1031,38 @@
       <c r="F11" s="5">
         <v>3.9216666666666669</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11">
         <v>2676</v>
       </c>
-      <c r="J11" s="8">
+      <c r="J11">
         <v>1</v>
       </c>
-      <c r="K11" s="9">
-        <f>K9+C43</f>
+      <c r="K11" s="8">
+        <f t="shared" ref="K11:P11" si="8">K9+C43</f>
         <v>0.3190972222222222</v>
       </c>
-      <c r="L11" s="9">
-        <f>L9+D43</f>
+      <c r="L11" s="8">
+        <f t="shared" si="8"/>
         <v>0.40914351851851843</v>
       </c>
-      <c r="M11" s="9">
-        <f>M9+E43</f>
+      <c r="M11" s="8">
+        <f t="shared" si="8"/>
         <v>0.49259259259259258</v>
       </c>
-      <c r="N11" s="9">
-        <f>N9+F43</f>
-        <v>0.52743055555555562</v>
-      </c>
-      <c r="O11" s="9">
-        <f>O9+G43</f>
+      <c r="N11" s="8">
+        <f t="shared" si="8"/>
+        <v>0.70798611111111109</v>
+      </c>
+      <c r="O11" s="8">
+        <f t="shared" si="8"/>
         <v>5.9027777777777776E-3</v>
       </c>
-      <c r="P11" s="9">
-        <f>P9+H43</f>
+      <c r="P11" s="8">
+        <f t="shared" si="8"/>
         <v>5.5555555555555558E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0.50347222222222221</v>
       </c>
@@ -1053,38 +1081,38 @@
       <c r="F12" s="5">
         <v>4.128571428571429</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12">
         <v>2677</v>
       </c>
-      <c r="J12" s="8">
-        <v>0</v>
-      </c>
-      <c r="K12" s="9">
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12" s="8">
         <f>K11+(K15-K11)*0.25</f>
         <v>0.32013888888888886</v>
       </c>
-      <c r="L12" s="9">
-        <f t="shared" ref="L12:P12" si="4">L11+(L15-L11)*0.25</f>
+      <c r="L12" s="8">
+        <f t="shared" ref="L12:P12" si="9">L11+(L15-L11)*0.25</f>
         <v>0.41001157407407396</v>
       </c>
-      <c r="M12" s="9">
-        <f t="shared" si="4"/>
+      <c r="M12" s="8">
+        <f t="shared" si="9"/>
         <v>0.49346064814814816</v>
       </c>
-      <c r="N12" s="9">
-        <f t="shared" si="4"/>
-        <v>0.5282986111111112</v>
-      </c>
-      <c r="O12" s="9">
-        <f t="shared" si="4"/>
+      <c r="N12" s="8">
+        <f t="shared" si="9"/>
+        <v>0.70885416666666667</v>
+      </c>
+      <c r="O12" s="8">
+        <f t="shared" si="9"/>
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="P12" s="9">
-        <f t="shared" si="4"/>
+      <c r="P12" s="8">
+        <f t="shared" si="9"/>
         <v>6.3368055555555556E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>0.52430555555555558</v>
       </c>
@@ -1103,38 +1131,38 @@
       <c r="F13" s="5">
         <v>4.1261904761904766</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13">
         <v>2678</v>
       </c>
-      <c r="J13" s="8">
-        <v>0</v>
-      </c>
-      <c r="K13" s="9">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8">
         <f>K11+(K15-K11)*0.5</f>
         <v>0.32118055555555552</v>
       </c>
-      <c r="L13" s="9">
-        <f t="shared" ref="L13:P13" si="5">L11+(L15-L11)*0.5</f>
+      <c r="L13" s="8">
+        <f t="shared" ref="L13:P13" si="10">L11+(L15-L11)*0.5</f>
         <v>0.41087962962962954</v>
       </c>
-      <c r="M13" s="9">
-        <f t="shared" si="5"/>
+      <c r="M13" s="8">
+        <f t="shared" si="10"/>
         <v>0.49432870370370369</v>
       </c>
-      <c r="N13" s="9">
-        <f t="shared" si="5"/>
-        <v>0.52916666666666679</v>
-      </c>
-      <c r="O13" s="9">
-        <f t="shared" si="5"/>
+      <c r="N13" s="8">
+        <f t="shared" si="10"/>
+        <v>0.70972222222222214</v>
+      </c>
+      <c r="O13" s="8">
+        <f t="shared" si="10"/>
         <v>7.9861111111111105E-3</v>
       </c>
-      <c r="P13" s="9">
-        <f t="shared" si="5"/>
+      <c r="P13" s="8">
+        <f t="shared" si="10"/>
         <v>7.1180555555555563E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>0.54513888888888895</v>
       </c>
@@ -1153,38 +1181,38 @@
       <c r="F14" s="5">
         <v>3.9645833333333331</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14">
         <v>2679</v>
       </c>
-      <c r="J14" s="8">
-        <v>0</v>
-      </c>
-      <c r="K14" s="9">
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="8">
         <f>K11+(K15-K11)*0.75</f>
         <v>0.32222222222222219</v>
       </c>
-      <c r="L14" s="9">
-        <f t="shared" ref="L14:P14" si="6">L11+(L15-L11)*0.75</f>
+      <c r="L14" s="8">
+        <f t="shared" ref="L14:P14" si="11">L11+(L15-L11)*0.75</f>
         <v>0.41174768518518512</v>
       </c>
-      <c r="M14" s="9">
-        <f t="shared" si="6"/>
+      <c r="M14" s="8">
+        <f t="shared" si="11"/>
         <v>0.49519675925925921</v>
       </c>
-      <c r="N14" s="9">
-        <f t="shared" si="6"/>
-        <v>0.53003472222222225</v>
-      </c>
-      <c r="O14" s="9">
-        <f t="shared" si="6"/>
+      <c r="N14" s="8">
+        <f t="shared" si="11"/>
+        <v>0.71059027777777772</v>
+      </c>
+      <c r="O14" s="8">
+        <f t="shared" si="11"/>
         <v>9.0277777777777769E-3</v>
       </c>
-      <c r="P14" s="9">
-        <f t="shared" si="6"/>
+      <c r="P14" s="8">
+        <f t="shared" si="11"/>
         <v>7.8993055555555552E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>0.56597222222222221</v>
       </c>
@@ -1203,38 +1231,38 @@
       <c r="F15" s="5">
         <v>3.837037037037037</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15">
         <v>2375</v>
       </c>
-      <c r="J15" s="8">
+      <c r="J15">
         <v>1</v>
       </c>
-      <c r="K15" s="9">
-        <f>K11+C44</f>
+      <c r="K15" s="8">
+        <f t="shared" ref="K15:P15" si="12">K11+C44</f>
         <v>0.32326388888888885</v>
       </c>
-      <c r="L15" s="9">
-        <f>L11+D44</f>
+      <c r="L15" s="8">
+        <f t="shared" si="12"/>
         <v>0.41261574074074064</v>
       </c>
-      <c r="M15" s="9">
-        <f>M11+E44</f>
+      <c r="M15" s="8">
+        <f t="shared" si="12"/>
         <v>0.49606481481481479</v>
       </c>
-      <c r="N15" s="9">
-        <f>N11+F44</f>
-        <v>0.53090277777777783</v>
-      </c>
-      <c r="O15" s="9">
-        <f>O11+G44</f>
+      <c r="N15" s="8">
+        <f t="shared" si="12"/>
+        <v>0.7114583333333333</v>
+      </c>
+      <c r="O15" s="8">
+        <f t="shared" si="12"/>
         <v>1.0069444444444443E-2</v>
       </c>
-      <c r="P15" s="9">
-        <f>P11+H44</f>
+      <c r="P15" s="8">
+        <f t="shared" si="12"/>
         <v>8.6805555555555559E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>0.58680555555555558</v>
       </c>
@@ -1253,11 +1281,8 @@
       <c r="F16" s="5">
         <v>4.4309523809523803</v>
       </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>0.60763888888888895</v>
       </c>
@@ -1276,11 +1301,8 @@
       <c r="F17" s="5">
         <v>4.0291666666666668</v>
       </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>0.62847222222222221</v>
       </c>
@@ -1299,11 +1321,8 @@
       <c r="F18" s="5">
         <v>3.9740740740740743</v>
       </c>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>0.64930555555555558</v>
       </c>
@@ -1323,7 +1342,7 @@
         <v>4.7555555555555555</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>0.67013888888888884</v>
       </c>
@@ -1343,7 +1362,7 @@
         <v>4.5740740740740744</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0.69097222222222221</v>
       </c>
@@ -1363,7 +1382,7 @@
         <v>4.2619047619047619</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>0.71180555555555547</v>
       </c>
@@ -1383,7 +1402,7 @@
         <v>3.6555555555555559</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>0.73263888888888884</v>
       </c>
@@ -1403,7 +1422,7 @@
         <v>3.7476190476190476</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>0.75347222222222221</v>
       </c>
@@ -1423,7 +1442,7 @@
         <v>3.8537037037037036</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>0.77430555555555547</v>
       </c>
@@ -1443,7 +1462,7 @@
         <v>3.835185185185185</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>0.81597222222222221</v>
       </c>
@@ -1463,7 +1482,7 @@
         <v>3.6018518518518521</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>0.85763888888888884</v>
       </c>
@@ -1483,7 +1502,7 @@
         <v>3.751851851851852</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>0.89930555555555547</v>
       </c>
@@ -1503,7 +1522,7 @@
         <v>3.4222222222222225</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>0.94097222222222221</v>
       </c>
@@ -1523,7 +1542,7 @@
         <v>3.3250000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>0.98263888888888884</v>
       </c>
@@ -1543,7 +1562,7 @@
         <v>3.2458333333333331</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -1563,7 +1582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>720</v>
       </c>
@@ -1584,7 +1603,7 @@
         <v>13.633333333333335</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>750</v>
       </c>
@@ -1601,11 +1620,11 @@
         <v>3.9099999999999997</v>
       </c>
       <c r="F34">
-        <f t="shared" ref="F34:F38" si="7">SUM(B34:E34)</f>
+        <f t="shared" ref="F34:F38" si="13">SUM(B34:E34)</f>
         <v>13.426666666666666</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>950</v>
       </c>
@@ -1622,11 +1641,11 @@
         <v>3.6666666666666665</v>
       </c>
       <c r="F35">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12.016666666666666</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1150</v>
       </c>
@@ -1643,11 +1662,11 @@
         <v>4.1966666666666672</v>
       </c>
       <c r="F36">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>13.146666666666667</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>1750</v>
       </c>
@@ -1664,11 +1683,11 @@
         <v>3.7433333333333332</v>
       </c>
       <c r="F37">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>12.04</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2250</v>
       </c>
@@ -1685,11 +1704,11 @@
         <v>3.4</v>
       </c>
       <c r="F38">
-        <f t="shared" si="7"/>
+        <f t="shared" si="13"/>
         <v>11.273333333333333</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>10</v>
       </c>
@@ -1712,128 +1731,380 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B41" s="10" t="s">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B41" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="11">
+      <c r="C41" s="8">
         <v>1.736111111111111E-3</v>
       </c>
-      <c r="D41" s="11">
+      <c r="D41" s="8">
         <v>1.8518518518518517E-3</v>
       </c>
-      <c r="E41" s="11">
+      <c r="E41" s="8">
         <v>1.736111111111111E-3</v>
       </c>
-      <c r="F41" s="11">
+      <c r="F41" s="8">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="G41" s="11">
+      <c r="G41" s="8">
         <v>1.736111111111111E-3</v>
       </c>
-      <c r="H41" s="11">
+      <c r="H41" s="8">
         <v>1.736111111111111E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B42" s="10" t="s">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="C42" s="11">
+      <c r="C42" s="8">
         <v>3.1249999999999997E-3</v>
       </c>
-      <c r="D42" s="11">
+      <c r="D42" s="8">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="E42" s="11">
+      <c r="E42" s="8">
         <v>2.6620370370370374E-3</v>
       </c>
-      <c r="F42" s="11">
+      <c r="F42" s="8">
         <v>2.7777777777777779E-3</v>
       </c>
-      <c r="G42" s="11">
+      <c r="G42" s="8">
         <v>2.4305555555555556E-3</v>
       </c>
-      <c r="H42" s="11">
+      <c r="H42" s="8">
         <v>2.4305555555555556E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B43" s="10" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C43" s="11">
+      <c r="C43" s="8">
         <v>1.736111111111111E-3</v>
       </c>
-      <c r="D43" s="11">
+      <c r="D43" s="8">
         <v>1.736111111111111E-3</v>
       </c>
-      <c r="E43" s="11">
+      <c r="E43" s="8">
         <v>2.0833333333333333E-3</v>
       </c>
-      <c r="F43" s="11">
+      <c r="F43" s="8">
         <v>1.736111111111111E-3</v>
       </c>
-      <c r="G43" s="11">
+      <c r="G43" s="8">
         <v>1.736111111111111E-3</v>
       </c>
-      <c r="H43" s="11">
+      <c r="H43" s="8">
         <v>1.3888888888888889E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B44" s="10" t="s">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="11">
+      <c r="C44" s="8">
         <v>4.1666666666666666E-3</v>
       </c>
-      <c r="D44" s="11">
+      <c r="D44" s="8">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="E44" s="11">
+      <c r="E44" s="8">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="F44" s="11">
+      <c r="F44" s="8">
         <v>3.472222222222222E-3</v>
       </c>
-      <c r="G44" s="11">
+      <c r="G44" s="8">
         <v>4.1666666666666666E-3</v>
       </c>
-      <c r="H44" s="11">
+      <c r="H44" s="8">
         <v>3.1249999999999997E-3</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B45" s="10" t="s">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="12">
+      <c r="C45" s="10">
         <f>SUM(C41:C44)</f>
         <v>1.0763888888888889E-2</v>
       </c>
-      <c r="D45" s="12">
-        <f t="shared" ref="D45:H45" si="8">SUM(D41:D44)</f>
+      <c r="D45" s="10">
+        <f t="shared" ref="D45:H45" si="14">SUM(D41:D44)</f>
         <v>9.8379629629629615E-3</v>
       </c>
-      <c r="E45" s="12">
-        <f t="shared" si="8"/>
+      <c r="E45" s="10">
+        <f t="shared" si="14"/>
         <v>9.9537037037037042E-3</v>
       </c>
-      <c r="F45" s="12">
-        <f t="shared" si="8"/>
+      <c r="F45" s="10">
+        <f t="shared" si="14"/>
         <v>1.0069444444444443E-2</v>
       </c>
-      <c r="G45" s="12">
-        <f t="shared" si="8"/>
+      <c r="G45" s="10">
+        <f t="shared" si="14"/>
         <v>1.0069444444444443E-2</v>
       </c>
-      <c r="H45" s="12">
-        <f t="shared" si="8"/>
+      <c r="H45" s="10">
+        <f t="shared" si="14"/>
         <v>8.6805555555555559E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" t="s">
+        <v>8</v>
+      </c>
+      <c r="G51" t="s">
+        <v>9</v>
+      </c>
+      <c r="H51" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="8">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="F52">
+        <v>1341</v>
+      </c>
+      <c r="G52">
+        <v>1</v>
+      </c>
+      <c r="H52" s="8">
+        <v>0.90277777777777779</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" s="8">
+        <v>1.736111111111111E-3</v>
+      </c>
+      <c r="F53">
+        <v>1342</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53" s="8">
+        <f>H52+(H57-H52)*0.2</f>
+        <v>0.90347222222222223</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="8">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="F54">
+        <v>2699</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+      <c r="H54" s="8">
+        <f>H52+(H57-H52)*0.4</f>
+        <v>0.90416666666666667</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="8">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="F55">
+        <v>1501</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55" s="8">
+        <f>H52+(H57-H52)*0.6</f>
+        <v>0.90486111111111112</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>19</v>
+      </c>
+      <c r="D56" s="10">
+        <f t="shared" ref="D56" si="15">SUM(D52:D55)</f>
+        <v>1.1458333333333333E-2</v>
+      </c>
+      <c r="F56">
+        <v>2101</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56" s="8">
+        <f>H52+(H57-H52)*0.8</f>
+        <v>0.90555555555555556</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>2102</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57" s="8">
+        <f>H52+D52</f>
+        <v>0.90625</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>1617</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58" s="8">
+        <f>H57+(H60-H57)*0.33</f>
+        <v>0.9068229166666667</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>1616</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59" s="8">
+        <f>H57+(H60-H57)*0.67</f>
+        <v>0.90741319444444446</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>1615</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60" s="8">
+        <f>H57+D53</f>
+        <v>0.90798611111111116</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>1509</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61" s="8">
+        <f>H60+(H64-H60)*0.25</f>
+        <v>0.9086805555555556</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F62">
+        <v>2448</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62" s="8">
+        <f>H60+(H64-H60)*0.5</f>
+        <v>0.90937500000000004</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F63">
+        <v>2516</v>
+      </c>
+      <c r="G63">
+        <v>0</v>
+      </c>
+      <c r="H63" s="8">
+        <f>H60+(H64-H60)*0.75</f>
+        <v>0.91006944444444449</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="F64">
+        <v>1505</v>
+      </c>
+      <c r="G64">
+        <v>1</v>
+      </c>
+      <c r="H64" s="8">
+        <f>H60+D54</f>
+        <v>0.91076388888888893</v>
+      </c>
+    </row>
+    <row r="65" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F65">
+        <v>2328</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65" s="8">
+        <f>H64+(H68-H64)*0.25</f>
+        <v>0.91163194444444451</v>
+      </c>
+    </row>
+    <row r="66" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F66">
+        <v>2739</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
+      <c r="H66" s="8">
+        <f>H64+(H68-H64)*0.5</f>
+        <v>0.91250000000000009</v>
+      </c>
+    </row>
+    <row r="67" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F67">
+        <v>1510</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67" s="8">
+        <f>H64+(H68-H64)*0.75</f>
+        <v>0.91336805555555556</v>
+      </c>
+    </row>
+    <row r="68" spans="6:8" x14ac:dyDescent="0.25">
+      <c r="F68">
+        <v>1341</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
+      <c r="H68" s="8">
+        <f>H64+D55</f>
+        <v>0.91423611111111114</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>